<commit_message>
new doc files : Seattle, Bangkok, San Paolo
</commit_message>
<xml_diff>
--- a/doc/Bangkok_WINTER_Oct2018_March2019_AM.xlsx
+++ b/doc/Bangkok_WINTER_Oct2018_March2019_AM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margheritataddei/Desktop/SolarUtils/SolarSpectra/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margheritataddei/Desktop/SolarUtils/SolarSpectra/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D4A6F61-372F-8546-AA49-120D46BF454D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDC53FA-EF74-7B4B-A166-F0B1C87F9487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16540" xr2:uid="{182810A2-71AE-9348-8D9E-6AD61A1E7911}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="Bangkok_WINTER_Oct2018_March2019_AM" localSheetId="0">Foglio1!$A$1:$C$4369</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{A9393651-4F39-0A48-B1D0-D73B1E94C08C}" name="Bangkok_WINTER_Oct2018_March2019_AM" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/margheritataddei/Desktop/SolarUtils/SolarSpectra/Bangkok_WINTER_Oct2018_March2019_AM.rtf" decimal="," thousands="." tab="0" comma="1">
+    <textPr sourceFile="/Users/margheritataddei/Desktop/SolarUtils/SolarSpectra/Bangkok_WINTER_Oct2018_March2019_AM.rtf" decimal="," thousands="." tab="0" comma="1">
       <textFields>
         <textField/>
       </textFields>

</xml_diff>